<commit_message>
new scripts + changes to old
</commit_message>
<xml_diff>
--- a/ScoreMatrix.xlsx
+++ b/ScoreMatrix.xlsx
@@ -118,7 +118,7 @@
     <t>Exact same as ultimate baseline except added nmatch_brand to what trains the model</t>
   </si>
   <si>
-    <t>9% boost to brand matches over 0, baseline model</t>
+    <t>7% boost to brand matches over 0, baseline model</t>
   </si>
 </sst>
 </file>
@@ -183,11 +183,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,7 +472,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,7 +493,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1"/>
@@ -505,7 +505,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -523,13 +523,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -538,8 +538,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8">
@@ -547,52 +547,52 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
+      <c r="A22" s="4"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
+      <c r="A23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fuzzy match and bullets have been successful so far
</commit_message>
<xml_diff>
--- a/ScoreMatrix.xlsx
+++ b/ScoreMatrix.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjvan\Documents\Kaggle\HomeDepot_early_2016\homedepotgit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="5415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="5420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +32,7 @@
     <author>Taylor Van Anne</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="1">
+    <comment ref="B7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Baseline</t>
   </si>
@@ -117,13 +122,22 @@
   </si>
   <si>
     <t>Baseline glm with added bullet count</t>
+  </si>
+  <si>
+    <t>baseline glm fuzzy match percents (normalized)</t>
+  </si>
+  <si>
+    <t>Baseline glm fuzzy match (raw)</t>
+  </si>
+  <si>
+    <t>add bullets to this and we're cooking with gas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,10 +198,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,30 +474,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="6" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -491,8 +505,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1"/>
@@ -503,17 +517,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.51146999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -521,14 +535,14 @@
         <v>0.51597000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -536,8 +550,8 @@
         <v>0.54698999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -545,59 +559,74 @@
         <v>0.54698999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>0.51053000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="4"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.50163999999999997</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.50014000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -610,24 +639,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>